<commit_message>
Update tools {props_config tool}
</commit_message>
<xml_diff>
--- a/props_config_tool/Props_config .xlsx
+++ b/props_config_tool/Props_config .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fotoable/Gamedev_Tools/props_config_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E477BAC7-9595-B34C-BCC1-7B2303693859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA88C39A-10D7-2742-BFB8-6AFF80FBB1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1860" yWindow="-21100" windowWidth="36520" windowHeight="21100" xr2:uid="{A31C8E30-1433-5E44-A4D4-D6FE9C517B26}"/>
+    <workbookView xWindow="-7580" yWindow="-26980" windowWidth="42920" windowHeight="23520" xr2:uid="{A31C8E30-1433-5E44-A4D4-D6FE9C517B26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -480,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD93D1C0-6563-2640-AF84-D98EFC162682}">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -616,6 +616,298 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:27">
+      <c r="A3" s="1">
+        <v>24800</v>
+      </c>
+      <c r="B3" s="1">
+        <v>24800</v>
+      </c>
+      <c r="D3" s="2">
+        <v>31</v>
+      </c>
+      <c r="E3" s="2">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2">
+        <v>38</v>
+      </c>
+      <c r="G3" s="2">
+        <v>6</v>
+      </c>
+      <c r="I3" s="3">
+        <v>31</v>
+      </c>
+      <c r="J3" s="3">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3">
+        <v>63</v>
+      </c>
+      <c r="L3" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" s="1">
+        <v>23900</v>
+      </c>
+      <c r="B4" s="1">
+        <v>23900</v>
+      </c>
+      <c r="D4" s="2">
+        <v>31</v>
+      </c>
+      <c r="E4" s="2">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2">
+        <v>63</v>
+      </c>
+      <c r="G4" s="2">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3">
+        <v>37</v>
+      </c>
+      <c r="J4" s="3">
+        <v>6</v>
+      </c>
+      <c r="K4" s="3">
+        <v>63</v>
+      </c>
+      <c r="L4" s="3">
+        <v>6</v>
+      </c>
+      <c r="N4" s="4">
+        <v>37</v>
+      </c>
+      <c r="O4" s="4">
+        <v>6</v>
+      </c>
+      <c r="P4" s="4">
+        <v>38</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>6</v>
+      </c>
+      <c r="S4" s="5">
+        <v>37</v>
+      </c>
+      <c r="T4" s="5">
+        <v>6</v>
+      </c>
+      <c r="U4" s="5">
+        <v>39</v>
+      </c>
+      <c r="V4" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" s="1">
+        <v>24200</v>
+      </c>
+      <c r="B5" s="1">
+        <v>24200</v>
+      </c>
+      <c r="D5" s="2">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2">
+        <v>38</v>
+      </c>
+      <c r="G5" s="2">
+        <v>6</v>
+      </c>
+      <c r="I5" s="3">
+        <v>37</v>
+      </c>
+      <c r="J5" s="3">
+        <v>6</v>
+      </c>
+      <c r="K5" s="3">
+        <v>63</v>
+      </c>
+      <c r="L5" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" s="1">
+        <v>24700</v>
+      </c>
+      <c r="B6" s="1">
+        <v>24700</v>
+      </c>
+      <c r="D6" s="2">
+        <v>31</v>
+      </c>
+      <c r="E6" s="2">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2">
+        <v>63</v>
+      </c>
+      <c r="G6" s="2">
+        <v>6</v>
+      </c>
+      <c r="I6" s="3">
+        <v>37</v>
+      </c>
+      <c r="J6" s="3">
+        <v>6</v>
+      </c>
+      <c r="K6" s="3">
+        <v>63</v>
+      </c>
+      <c r="L6" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" s="1">
+        <v>24600</v>
+      </c>
+      <c r="B7" s="1">
+        <v>24600</v>
+      </c>
+      <c r="D7" s="2">
+        <v>31</v>
+      </c>
+      <c r="E7" s="2">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2">
+        <v>63</v>
+      </c>
+      <c r="G7" s="2">
+        <v>6</v>
+      </c>
+      <c r="I7" s="3">
+        <v>37</v>
+      </c>
+      <c r="J7" s="3">
+        <v>6</v>
+      </c>
+      <c r="K7" s="3">
+        <v>38</v>
+      </c>
+      <c r="L7" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" s="1">
+        <v>24000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>24000</v>
+      </c>
+      <c r="D8" s="2">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2">
+        <v>38</v>
+      </c>
+      <c r="G8" s="2">
+        <v>6</v>
+      </c>
+      <c r="I8" s="3">
+        <v>37</v>
+      </c>
+      <c r="J8" s="3">
+        <v>6</v>
+      </c>
+      <c r="K8" s="3">
+        <v>63</v>
+      </c>
+      <c r="L8" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" s="1">
+        <v>23800</v>
+      </c>
+      <c r="B9" s="1">
+        <v>23800</v>
+      </c>
+      <c r="D9" s="2">
+        <v>31</v>
+      </c>
+      <c r="E9" s="2">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2">
+        <v>63</v>
+      </c>
+      <c r="G9" s="2">
+        <v>6</v>
+      </c>
+      <c r="I9" s="3">
+        <v>37</v>
+      </c>
+      <c r="J9" s="3">
+        <v>6</v>
+      </c>
+      <c r="K9" s="3">
+        <v>63</v>
+      </c>
+      <c r="L9" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="A10" s="1">
+        <v>24300</v>
+      </c>
+      <c r="B10" s="1">
+        <v>24300</v>
+      </c>
+      <c r="D10" s="2">
+        <v>31</v>
+      </c>
+      <c r="E10" s="2">
+        <v>11</v>
+      </c>
+      <c r="F10" s="2">
+        <v>63</v>
+      </c>
+      <c r="G10" s="2">
+        <v>6</v>
+      </c>
+      <c r="I10" s="3">
+        <v>37</v>
+      </c>
+      <c r="J10" s="3">
+        <v>6</v>
+      </c>
+      <c r="K10" s="3">
+        <v>63</v>
+      </c>
+      <c r="L10" s="3">
+        <v>6</v>
+      </c>
+      <c r="N10" s="4">
+        <v>31</v>
+      </c>
+      <c r="O10" s="4">
+        <v>11</v>
+      </c>
+      <c r="P10" s="4">
+        <v>38</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C1:G1"/>

</xml_diff>

<commit_message>
Update new config tools
</commit_message>
<xml_diff>
--- a/props_config_tool/Props_config .xlsx
+++ b/props_config_tool/Props_config .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fotoable/Gamedev_Tools/props_config_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA88C39A-10D7-2742-BFB8-6AFF80FBB1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCE204F-94AA-4F4D-AD09-78E37A3C99FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-7580" yWindow="-26980" windowWidth="42920" windowHeight="23520" xr2:uid="{A31C8E30-1433-5E44-A4D4-D6FE9C517B26}"/>
   </bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>

</xml_diff>